<commit_message>
laravel installed; DB cofings...
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -357,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -491,6 +491,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,10 +813,10 @@
   <dimension ref="A1:IK71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="L5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AI15" sqref="AI15"/>
+      <selection pane="bottomRight" activeCell="AC10" sqref="AC10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="22.5" customHeight="1"/>
@@ -1422,7 +1425,7 @@
       <c r="M7" s="30"/>
     </row>
     <row r="8" spans="1:245" ht="22.5" customHeight="1">
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="29" t="s">
         <v>9</v>
       </c>
       <c r="T8" s="22"/>
@@ -1508,7 +1511,7 @@
       <c r="C12" s="28"/>
     </row>
     <row r="14" spans="1:245" ht="22.5" customHeight="1">
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="52" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="22"/>
@@ -1524,7 +1527,7 @@
       <c r="AC14" s="30"/>
     </row>
     <row r="15" spans="1:245" ht="22.5" customHeight="1">
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="52" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="22"/>
@@ -1539,13 +1542,27 @@
       <c r="AC15" s="6"/>
       <c r="AF15" s="22"/>
       <c r="AG15" s="30"/>
+      <c r="AJ15" s="22"/>
+      <c r="AK15" s="30"/>
+      <c r="AL15" s="30"/>
+      <c r="AN15" s="5"/>
+      <c r="AO15" s="6"/>
+      <c r="AP15" s="6"/>
+      <c r="AQ15" s="6"/>
+      <c r="AV15" s="22"/>
+      <c r="AW15" s="30"/>
+      <c r="AZ15" s="22"/>
     </row>
     <row r="16" spans="1:245" ht="22.5" customHeight="1">
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="57" t="s">
         <v>22</v>
       </c>
       <c r="X16" s="24"/>
       <c r="Y16" s="25"/>
+      <c r="AN16" s="22"/>
+      <c r="AO16" s="30"/>
+      <c r="AP16" s="30"/>
+      <c r="AQ16" s="30"/>
     </row>
     <row r="17" spans="1:172" ht="22.5" customHeight="1">
       <c r="A17" s="38"/>
@@ -1553,28 +1570,31 @@
     </row>
     <row r="18" spans="1:172" ht="22.5" customHeight="1">
       <c r="A18" s="39"/>
-      <c r="C18" s="53" t="s">
+      <c r="C18" s="57" t="s">
         <v>35</v>
       </c>
       <c r="O18" s="30"/>
       <c r="Z18" s="25"/>
       <c r="AA18" s="25"/>
+      <c r="BA18" s="30"/>
     </row>
     <row r="19" spans="1:172" ht="22.5" customHeight="1">
       <c r="A19" s="39"/>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="57" t="s">
         <v>36</v>
       </c>
       <c r="AB19" s="24"/>
       <c r="AC19" s="25"/>
+      <c r="BA19" s="30"/>
     </row>
     <row r="20" spans="1:172" ht="22.5" customHeight="1">
       <c r="A20" s="39"/>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="57" t="s">
         <v>37</v>
       </c>
       <c r="AD20" s="25"/>
       <c r="AE20" s="25"/>
+      <c r="BA20" s="30"/>
     </row>
     <row r="21" spans="1:172" ht="22.5" customHeight="1">
       <c r="C21" s="28"/>
@@ -1613,10 +1633,10 @@
       <c r="BG23" s="56"/>
     </row>
     <row r="24" spans="1:172" ht="22.5" customHeight="1">
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AN24" s="24"/>
+      <c r="AN24" s="22"/>
       <c r="AO24" s="25"/>
     </row>
     <row r="25" spans="1:172" s="6" customFormat="1" ht="22.5" customHeight="1">
@@ -1684,7 +1704,7 @@
       <c r="AM26" s="25"/>
     </row>
     <row r="27" spans="1:172" ht="22.5" customHeight="1">
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="53" t="s">
         <v>40</v>
       </c>
       <c r="AN27" s="24"/>
@@ -1697,7 +1717,7 @@
       <c r="AU27" s="25"/>
     </row>
     <row r="28" spans="1:172" ht="22.5" customHeight="1">
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="53" t="s">
         <v>57</v>
       </c>
       <c r="AV28" s="24"/>
@@ -1706,7 +1726,7 @@
       <c r="AY28" s="25"/>
     </row>
     <row r="29" spans="1:172" ht="22.5" customHeight="1">
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="53" t="s">
         <v>41</v>
       </c>
       <c r="AZ29" s="24"/>

</xml_diff>

<commit_message>
html, product table, form
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -351,7 +351,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -377,11 +377,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -521,53 +530,28 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -882,10 +866,10 @@
   <dimension ref="A1:IO77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="BB14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="BL20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="BF26" sqref="BF26"/>
+      <selection pane="bottomRight" activeCell="C40" sqref="C39:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="22.5" customHeight="1"/>
@@ -907,6 +891,7 @@
     <col min="44" max="44" width="3.7109375" style="1" customWidth="1"/>
     <col min="48" max="48" width="3.7109375" style="1" customWidth="1"/>
     <col min="52" max="52" width="3.7109375" style="1" customWidth="1"/>
+    <col min="56" max="56" width="3.7109375" style="64"/>
     <col min="60" max="60" width="3.7109375" style="1" customWidth="1"/>
     <col min="64" max="64" width="3.7109375" style="1" customWidth="1"/>
     <col min="68" max="68" width="3.7109375" style="1" customWidth="1"/>
@@ -1035,20 +1020,20 @@
       </c>
       <c r="BA1" s="58"/>
       <c r="BB1" s="12"/>
-      <c r="BC1" s="58"/>
-      <c r="BD1" s="12"/>
-      <c r="BE1" s="58"/>
-      <c r="BF1" s="12"/>
-      <c r="BG1" s="58"/>
-      <c r="BH1" s="13">
+      <c r="BC1" s="60"/>
+      <c r="BD1" s="61">
         <f>SUM(AZ1)+1</f>
         <v>7</v>
       </c>
-      <c r="BI1" s="14"/>
+      <c r="BE1" s="59"/>
+      <c r="BF1" s="14"/>
+      <c r="BG1" s="59"/>
+      <c r="BH1" s="14"/>
+      <c r="BI1" s="59"/>
       <c r="BJ1" s="14"/>
       <c r="BK1" s="14"/>
       <c r="BL1" s="9">
-        <f>SUM(BH1)+1</f>
+        <f>SUM(BD1)+1</f>
         <v>8</v>
       </c>
       <c r="BM1" s="21"/>
@@ -1272,6 +1257,7 @@
       <c r="AR2" s="15"/>
       <c r="AV2" s="15"/>
       <c r="AZ2" s="15"/>
+      <c r="BD2" s="62"/>
       <c r="BH2" s="15"/>
       <c r="BJ2" s="20"/>
       <c r="BL2" s="15"/>
@@ -1326,6 +1312,7 @@
       <c r="AR3" s="15"/>
       <c r="AV3" s="15"/>
       <c r="AZ3" s="15"/>
+      <c r="BD3" s="62"/>
       <c r="BH3" s="15"/>
       <c r="BL3" s="15"/>
       <c r="BP3" s="15"/>
@@ -1379,6 +1366,7 @@
       <c r="AR4" s="5"/>
       <c r="AV4" s="5"/>
       <c r="AZ4" s="5"/>
+      <c r="BD4" s="63"/>
       <c r="BH4" s="5"/>
       <c r="BL4" s="5"/>
       <c r="BP4" s="5"/>
@@ -1452,6 +1440,7 @@
       <c r="AR5" s="5"/>
       <c r="AV5" s="5"/>
       <c r="AZ5" s="5"/>
+      <c r="BD5" s="63"/>
       <c r="BH5" s="5"/>
       <c r="BL5" s="5"/>
       <c r="BP5" s="5"/>
@@ -1524,6 +1513,7 @@
       <c r="AR9" s="5"/>
       <c r="AV9" s="5"/>
       <c r="AZ9" s="5"/>
+      <c r="BD9" s="63"/>
       <c r="BH9" s="5"/>
       <c r="BL9" s="5"/>
       <c r="BP9" s="5"/>
@@ -1642,7 +1632,7 @@
       <c r="C17" s="38"/>
       <c r="BB17" s="6"/>
       <c r="BC17" s="6"/>
-      <c r="BD17" s="6"/>
+      <c r="BD17" s="63"/>
       <c r="BE17" s="6"/>
       <c r="BF17" s="6"/>
       <c r="BG17" s="6"/>
@@ -1658,7 +1648,7 @@
       <c r="BA18" s="30"/>
       <c r="BB18" s="6"/>
       <c r="BC18" s="6"/>
-      <c r="BD18" s="6"/>
+      <c r="BD18" s="63"/>
       <c r="BE18" s="6"/>
       <c r="BF18" s="6"/>
       <c r="BG18" s="6"/>
@@ -1673,7 +1663,7 @@
       <c r="BA19" s="30"/>
       <c r="BB19" s="6"/>
       <c r="BC19" s="6"/>
-      <c r="BD19" s="6"/>
+      <c r="BD19" s="63"/>
       <c r="BE19" s="6"/>
       <c r="BF19" s="6"/>
       <c r="BG19" s="6"/>
@@ -1688,7 +1678,7 @@
       <c r="BA20" s="30"/>
       <c r="BB20" s="30"/>
       <c r="BC20" s="6"/>
-      <c r="BD20" s="6"/>
+      <c r="BD20" s="63"/>
       <c r="BE20" s="6"/>
       <c r="BF20" s="6"/>
       <c r="BG20" s="6"/>
@@ -1697,7 +1687,7 @@
       <c r="C21" s="28"/>
       <c r="BB21" s="6"/>
       <c r="BC21" s="6"/>
-      <c r="BD21" s="6"/>
+      <c r="BD21" s="63"/>
       <c r="BE21" s="6"/>
       <c r="BF21" s="6"/>
       <c r="BG21" s="6"/>
@@ -1730,7 +1720,7 @@
       <c r="BA23" s="55"/>
       <c r="BB23" s="55"/>
       <c r="BC23" s="55"/>
-      <c r="BD23" s="55"/>
+      <c r="BD23" s="65"/>
       <c r="BE23" s="55"/>
       <c r="BF23" s="55"/>
       <c r="BG23" s="55"/>
@@ -1766,6 +1756,7 @@
       <c r="AR25" s="5"/>
       <c r="AV25" s="5"/>
       <c r="AZ25" s="5"/>
+      <c r="BD25" s="63"/>
       <c r="BH25" s="5"/>
       <c r="BL25" s="5"/>
       <c r="BP25" s="5"/>
@@ -1809,9 +1800,17 @@
       <c r="AK26" s="25"/>
       <c r="AL26" s="25"/>
       <c r="AM26" s="25"/>
-      <c r="BC26" s="30"/>
-      <c r="BD26" s="30"/>
+      <c r="BC26" s="6"/>
+      <c r="BD26" s="66"/>
       <c r="BE26" s="30"/>
+      <c r="BF26" s="30"/>
+      <c r="BG26" s="30"/>
+      <c r="BH26" s="22"/>
+      <c r="BI26" s="30"/>
+      <c r="BJ26" s="30"/>
+      <c r="BK26" s="30"/>
+      <c r="BP26" s="22"/>
+      <c r="BQ26" s="30"/>
     </row>
     <row r="27" spans="1:176" ht="22.5" customHeight="1">
       <c r="C27" s="56" t="s">
@@ -1826,7 +1825,7 @@
       <c r="AL27" s="25"/>
       <c r="AM27" s="25"/>
       <c r="BC27" s="6"/>
-      <c r="BD27" s="6"/>
+      <c r="BD27" s="63"/>
       <c r="BE27" s="6"/>
     </row>
     <row r="28" spans="1:176" ht="22.5" customHeight="1">
@@ -1842,7 +1841,7 @@
       <c r="AL28" s="25"/>
       <c r="AM28" s="25"/>
       <c r="BC28" s="6"/>
-      <c r="BD28" s="6"/>
+      <c r="BD28" s="63"/>
       <c r="BE28" s="6"/>
     </row>
     <row r="29" spans="1:176" ht="22.5" customHeight="1">
@@ -1858,7 +1857,7 @@
       <c r="AL29" s="25"/>
       <c r="AM29" s="25"/>
       <c r="BC29" s="6"/>
-      <c r="BD29" s="6"/>
+      <c r="BD29" s="63"/>
       <c r="BE29" s="6"/>
     </row>
     <row r="30" spans="1:176" ht="22.5" customHeight="1">
@@ -1874,7 +1873,7 @@
       <c r="AL30" s="25"/>
       <c r="AM30" s="25"/>
       <c r="BC30" s="6"/>
-      <c r="BD30" s="6"/>
+      <c r="BD30" s="63"/>
       <c r="BE30" s="6"/>
     </row>
     <row r="31" spans="1:176" ht="22.5" customHeight="1">
@@ -1890,7 +1889,7 @@
       <c r="AL31" s="25"/>
       <c r="AM31" s="25"/>
       <c r="BC31" s="6"/>
-      <c r="BD31" s="6"/>
+      <c r="BD31" s="63"/>
       <c r="BE31" s="6"/>
     </row>
     <row r="32" spans="1:176" ht="22.5" customHeight="1">
@@ -1906,7 +1905,7 @@
       <c r="AL32" s="25"/>
       <c r="AM32" s="25"/>
       <c r="BC32" s="6"/>
-      <c r="BD32" s="6"/>
+      <c r="BD32" s="63"/>
       <c r="BE32" s="6"/>
     </row>
     <row r="33" spans="1:176" ht="22.5" customHeight="1">
@@ -1936,7 +1935,7 @@
       <c r="BA35" s="25"/>
       <c r="BB35" s="25"/>
       <c r="BC35" s="25"/>
-      <c r="BD35" s="25"/>
+      <c r="BD35" s="67"/>
       <c r="BE35" s="25"/>
       <c r="BF35" s="25"/>
       <c r="BG35" s="25"/>
@@ -1949,26 +1948,34 @@
         <v>42</v>
       </c>
       <c r="BE37" s="30"/>
-      <c r="BH37" s="24"/>
-      <c r="BI37" s="25"/>
+      <c r="BF37" s="30"/>
+      <c r="BG37" s="30"/>
+      <c r="BH37" s="22"/>
+      <c r="BI37" s="30"/>
+      <c r="BJ37" s="30"/>
+      <c r="BK37" s="30"/>
     </row>
     <row r="38" spans="1:176" ht="22.5" customHeight="1">
       <c r="C38" s="56" t="s">
         <v>43</v>
       </c>
       <c r="BE38" s="30"/>
-      <c r="BJ38" s="25"/>
-      <c r="BK38" s="25"/>
+      <c r="BF38" s="30"/>
+      <c r="BG38" s="30"/>
+      <c r="BH38" s="22"/>
+      <c r="BI38" s="30"/>
+      <c r="BJ38" s="30"/>
+      <c r="BK38" s="30"/>
     </row>
     <row r="39" spans="1:176" ht="22.5" customHeight="1">
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="52" t="s">
         <v>44</v>
       </c>
       <c r="BL39" s="24"/>
       <c r="BM39" s="25"/>
     </row>
     <row r="40" spans="1:176" ht="22.5" customHeight="1">
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="52" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2010,10 +2017,10 @@
       <c r="CN42" s="5"/>
     </row>
     <row r="43" spans="1:176" ht="22.5" customHeight="1">
-      <c r="C43" s="40" t="s">
+      <c r="C43" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="BT43" s="24"/>
+      <c r="BT43" s="22"/>
       <c r="BU43" s="25"/>
     </row>
     <row r="44" spans="1:176" ht="22.5" customHeight="1">
@@ -2043,6 +2050,7 @@
       <c r="AR45" s="5"/>
       <c r="AV45" s="5"/>
       <c r="AZ45" s="5"/>
+      <c r="BD45" s="63"/>
       <c r="BH45" s="5"/>
       <c r="BL45" s="5"/>
       <c r="BP45" s="5"/>
@@ -2075,7 +2083,7 @@
       <c r="FT45" s="5"/>
     </row>
     <row r="46" spans="1:176" ht="22.5" customHeight="1">
-      <c r="C46" s="28" t="s">
+      <c r="C46" s="52" t="s">
         <v>25</v>
       </c>
       <c r="BL46" s="24"/>
@@ -2109,7 +2117,7 @@
       <c r="CN46" s="5"/>
     </row>
     <row r="47" spans="1:176" ht="22.5" customHeight="1">
-      <c r="C47" s="28" t="s">
+      <c r="C47" s="52" t="s">
         <v>26</v>
       </c>
       <c r="BL47" s="5"/>
@@ -2212,7 +2220,9 @@
       <c r="C50" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="BE50" s="30"/>
+      <c r="BI50" s="30"/>
+      <c r="BJ50" s="30"/>
+      <c r="BK50" s="30"/>
       <c r="BL50" s="5"/>
       <c r="BM50" s="6"/>
       <c r="BN50" s="6"/>
@@ -2247,7 +2257,9 @@
       <c r="C51" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="BE51" s="30"/>
+      <c r="BI51" s="30"/>
+      <c r="BJ51" s="30"/>
+      <c r="BK51" s="30"/>
       <c r="BL51" s="5"/>
       <c r="BM51" s="6"/>
       <c r="BN51" s="6"/>
@@ -2653,6 +2665,7 @@
       <c r="AR65" s="5"/>
       <c r="AV65" s="5"/>
       <c r="AZ65" s="5"/>
+      <c r="BD65" s="63"/>
       <c r="BH65" s="5"/>
       <c r="BL65" s="5"/>
       <c r="BP65" s="5"/>
@@ -2715,6 +2728,7 @@
       <c r="AR66" s="5"/>
       <c r="AV66" s="5"/>
       <c r="AZ66" s="5"/>
+      <c r="BD66" s="63"/>
       <c r="BH66" s="5"/>
       <c r="BL66" s="5"/>
       <c r="BP66" s="5"/>
@@ -2774,6 +2788,7 @@
       <c r="AR67" s="5"/>
       <c r="AV67" s="5"/>
       <c r="AZ67" s="5"/>
+      <c r="BD67" s="63"/>
       <c r="BH67" s="5"/>
       <c r="BL67" s="5"/>
       <c r="BP67" s="5"/>
@@ -2831,6 +2846,7 @@
       <c r="AR68" s="5"/>
       <c r="AV68" s="5"/>
       <c r="AZ68" s="5"/>
+      <c r="BD68" s="63"/>
       <c r="BH68" s="5"/>
       <c r="BL68" s="5"/>
       <c r="BP68" s="5"/>
@@ -2882,6 +2898,7 @@
       <c r="AR69" s="5"/>
       <c r="AV69" s="5"/>
       <c r="AZ69" s="5"/>
+      <c r="BD69" s="63"/>
       <c r="BH69" s="5"/>
       <c r="BL69" s="5"/>
       <c r="BP69" s="5"/>
@@ -2976,6 +2993,7 @@
       <c r="AR71" s="5"/>
       <c r="AV71" s="5"/>
       <c r="AZ71" s="5"/>
+      <c r="BD71" s="63"/>
       <c r="BH71" s="5"/>
       <c r="BL71" s="5"/>
       <c r="BP71" s="5"/>
@@ -3032,6 +3050,7 @@
       <c r="AR72" s="5"/>
       <c r="AV72" s="5"/>
       <c r="AZ72" s="5"/>
+      <c r="BD72" s="63"/>
       <c r="BH72" s="5"/>
       <c r="BL72" s="5"/>
       <c r="BP72" s="5"/>
@@ -3091,6 +3110,7 @@
       <c r="AR73" s="5"/>
       <c r="AV73" s="5"/>
       <c r="AZ73" s="5"/>
+      <c r="BD73" s="63"/>
       <c r="BH73" s="5"/>
       <c r="BL73" s="5"/>
       <c r="BP73" s="5"/>
@@ -3153,6 +3173,7 @@
       <c r="AR74" s="5"/>
       <c r="AV74" s="5"/>
       <c r="AZ74" s="5"/>
+      <c r="BD74" s="63"/>
       <c r="BH74" s="5"/>
       <c r="BL74" s="5"/>
       <c r="BP74" s="5"/>
@@ -3207,6 +3228,7 @@
       <c r="AR75" s="5"/>
       <c r="AV75" s="5"/>
       <c r="AZ75" s="5"/>
+      <c r="BD75" s="63"/>
       <c r="BH75" s="5"/>
       <c r="BL75" s="5"/>
       <c r="BP75" s="5"/>
@@ -3260,6 +3282,7 @@
       <c r="AR76" s="5"/>
       <c r="AV76" s="5"/>
       <c r="AZ76" s="5"/>
+      <c r="BD76" s="63"/>
       <c r="BH76" s="5"/>
       <c r="BL76" s="5"/>
       <c r="BP76" s="5"/>
@@ -3305,7 +3328,7 @@
       <c r="FT77" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="BL3 BP3 BT3 CB1:FT1 D1:CA2">
+  <conditionalFormatting sqref="BL3 BP3 BT3 CB1:FT1 BI1:CA2 BH2 D1:BG2">
     <cfRule type="cellIs" dxfId="2" priority="50" operator="equal">
       <formula>"/2=0"</formula>
     </cfRule>
@@ -3313,7 +3336,7 @@
       <formula>"/2"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:FT1">
+  <conditionalFormatting sqref="BI1:FT1 D1:BG1">
     <cfRule type="expression" dxfId="0" priority="49">
       <formula>ISODD(+$D$1)</formula>
     </cfRule>

</xml_diff>